<commit_message>
Add CRUD Bank API to api.py
</commit_message>
<xml_diff>
--- a/bank/bukti_matching/bni_matching.xlsx
+++ b/bank/bukti_matching/bni_matching.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,7 +502,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45535</v>
+        <v>45443</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -516,11 +516,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>330.025.845,00</t>
+          <t>148.943.002,00</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45535</v>
+        <v>45443</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -534,7 +534,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>330.025.845,00</t>
+          <t>148.943.002,00</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -556,11 +556,11 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45538</v>
+        <v>45447</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>236.327.692,00</t>
+          <t>114.574.866,00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -570,11 +570,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>566.353.537,00</t>
+          <t>263.517.868,00</t>
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45538</v>
+        <v>45447</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -583,12 +583,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>236.327.692,00</t>
+          <t>114.574.866,00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>566.353.537,00</t>
+          <t>263.517.868,00</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -614,7 +614,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45548</v>
+        <v>45473</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -623,18 +623,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>150.025.000,00</t>
+          <t>36.709,00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>416.328.537,00</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>263.481.159,00</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>45473</v>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>36.709,00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -644,7 +646,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>566.353.537,00</t>
+          <t>263.481.159,00</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -654,22 +656,24 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>150.025.000,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Unmatched</t>
+          <t>Matched</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>G1</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" s="2" t="n">
+        <v>45473</v>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>0,00</t>
@@ -677,20 +681,20 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>12.000,00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>416.328.537,00</t>
+          <t>263.469.159,00</t>
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>45548</v>
+        <v>45473</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>150.000.000,00</t>
+          <t>12.000,00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -700,7 +704,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>416.353.537,00</t>
+          <t>263.469.159,00</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -710,22 +714,24 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>-150.000.000,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Unmatched</t>
+          <t>Matched</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>G1</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" s="2" t="n">
+        <v>45473</v>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>0,00</t>
@@ -733,20 +739,20 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>10.000,00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>416.328.537,00</t>
+          <t>263.459.159,00</t>
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>45548</v>
+        <v>45473</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>25.000,00</t>
+          <t>10.000,00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -756,7 +762,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>416.328.537,00</t>
+          <t>263.459.159,00</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -766,27 +772,27 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>-25.000,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Unmatched</t>
+          <t>Matched</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>G1</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45565</v>
+        <v>45473</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>354.932,00</t>
+          <t>183.543,00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -796,11 +802,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>416.683.469,00</t>
+          <t>263.642.702,00</t>
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>45565</v>
+        <v>45473</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -809,12 +815,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>354.932,00</t>
+          <t>183.543,00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>416.683.469,00</t>
+          <t>263.642.702,00</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -840,39 +846,39 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45565</v>
+        <v>45473</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>114.758.409,00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>70.987,00</t>
+          <t>58.709,00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>416.612.482,00</t>
+          <t>263.642.702,00</t>
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>45565</v>
+        <v>45473</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>70.987,00</t>
+          <t>58.709,00</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>114.758.409,00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>416.612.482,00</t>
+          <t>263.642.702,00</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -887,184 +893,10 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Matched</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>45565</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>12.000,00</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>416.600.482,00</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>45565</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>12.000,00</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>416.600.482,00</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Matched</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>45565</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>10.000,00</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>416.590.482,00</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>45565</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>10.000,00</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>416.590.482,00</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Matched</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>45565</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>236.682.624,00</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>150.117.987,00</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>416.590.482,00</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>45565</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>150.117.987,00</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>236.682.624,00</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>416.590.482,00</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
           <t>Closing Balance</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1119,16 +951,16 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45535</v>
+        <v>45443</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>330.025.845,00</t>
+          <t>148.943.002,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>330.025.845,00</t>
+          <t>148.943.002,00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1144,16 +976,16 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45565</v>
+        <v>45473</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>416.590.482,00</t>
+          <t>263.642.702,00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>416.590.482,00</t>
+          <t>263.642.702,00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">

</xml_diff>